<commit_message>
Fixed Main Admin Filter Export and Adjusted Librarian Export too
</commit_message>
<xml_diff>
--- a/public/storage/department-admin-report.xlsx
+++ b/public/storage/department-admin-report.xlsx
@@ -131,12 +131,12 @@
     <row r="2" spans="1:7" customHeight="0">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>C001</t>
+          <t>R001</t>
         </is>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>Pan Doe</t>
+          <t>John Doe</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
@@ -156,11 +156,221 @@
       </c>
       <c r="F2" s="0" t="inlineStr">
         <is>
-          <t>2023-04-30 22:10:50</t>
+          <t>2023-04-21 14:07:35</t>
         </is>
       </c>
       <c r="G2" s="0">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" customHeight="0">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>R002</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>Jane Doe</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>College</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>Bachelor of Science in Information Technology</t>
+        </is>
+      </c>
+      <c r="E3" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="F3" s="0" t="inlineStr">
+        <is>
+          <t>2023-04-21 14:16:39</t>
+        </is>
+      </c>
+      <c r="G3" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" customHeight="0">
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>R003</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>Frank Doe</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>Senior High School</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>Accountancy, Business, and Management Strand</t>
+        </is>
+      </c>
+      <c r="E4" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="F4" s="0" t="inlineStr">
+        <is>
+          <t>2023-04-21 14:18:33</t>
+        </is>
+      </c>
+      <c r="G4" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" customHeight="0">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>R004</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>Hank Doe</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>Junior High School</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>Junior High School</t>
+        </is>
+      </c>
+      <c r="E5" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="F5" s="0" t="inlineStr">
+        <is>
+          <t>2023-04-21 14:19:30</t>
+        </is>
+      </c>
+      <c r="G5" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" customHeight="0">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>R005</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>Sam Doe</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>Graduate School</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>Master</t>
+        </is>
+      </c>
+      <c r="E6" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="F6" s="0" t="inlineStr">
+        <is>
+          <t>2023-04-21 14:41:02</t>
+        </is>
+      </c>
+      <c r="G6" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" customHeight="0">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>R001</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>Frank Doe</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>College</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>Bachelor of Science in Information Technology</t>
+        </is>
+      </c>
+      <c r="E7" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="F7" s="0" t="inlineStr">
+        <is>
+          <t>2023-05-27 11:00:59</t>
+        </is>
+      </c>
+      <c r="G7" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" customHeight="0">
+      <c r="A8" s="0" t="inlineStr">
+        <is>
+          <t>R001</t>
+        </is>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>Sam Smith</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>Graduate School</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>Master</t>
+        </is>
+      </c>
+      <c r="E8" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="F8" s="0" t="inlineStr">
+        <is>
+          <t>2023-05-01 10:03:29</t>
+        </is>
+      </c>
+      <c r="G8" s="0">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -171,37 +381,17 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetData>
-    <row r="1" spans="1:3" customHeight="0">
+    <row r="1" spans="1:1" customHeight="0">
       <c r="A1" s="0" t="inlineStr">
         <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" s="0" t="inlineStr">
-        <is>
-          <t>Department</t>
-        </is>
-      </c>
-      <c r="C1" s="0" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" spans="1:3" customHeight="0">
+          <t>Message</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" spans="1:1" customHeight="0">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>Jermey Tremblay II</t>
-        </is>
-      </c>
-      <c r="B2" s="0" t="inlineStr">
-        <is>
-          <t>Cashier</t>
-        </is>
-      </c>
-      <c r="C2" s="0" t="inlineStr">
-        <is>
-          <t>Logged Out</t>
+          <t>No data found within the specified date range.</t>
         </is>
       </c>
     </row>
@@ -222,7 +412,7 @@
     </row>
     <row r="2" spans="1:1" customHeight="0">
       <c r="A2" s="0">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -248,7 +438,7 @@
     <row r="3" spans="1:2" customHeight="0">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>Cashier</t>
+          <t>Registrar</t>
         </is>
       </c>
       <c r="B3" s="0">

</xml_diff>